<commit_message>
Refactor backtesting logic and enhance visualization features
- Updated backtesting.py to improve portfolio value calculation and streamline the backtesting process.
- Enhanced cointegration.py with better handling of correlation and cointegration tests.
- Modified main.py to use new tickers and simplify data processing.
- Expanded main_trials.py to include additional tickers for pair selection.
- Improved prints.py to provide more detailed results and metrics after backtesting.
- Enhanced visualization.py with new plotting functions for dynamic hedge ratios, trading signals, and portfolio splits.
- Removed unnecessary code and improved code readability across multiple files.
</commit_message>
<xml_diff>
--- a/004 tables.xlsx
+++ b/004 tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ppmel\Documentos\ITESO 7mo Semestre\004-Kalman-Filter-Implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ACDD3F-5464-4765-A4D5-7119A8A5B71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCDE9B8-E04A-44CE-AF95-3293A647CCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{920A4843-AD7D-4180-9CF4-44E3616DB8A7}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{920A4843-AD7D-4180-9CF4-44E3616DB8A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
   <si>
     <t>PAIR SELECTION</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Avg Win</t>
   </si>
   <si>
-    <t>Return</t>
-  </si>
-  <si>
     <t>TRAIN -TRADE STATISTICS</t>
   </si>
   <si>
@@ -180,6 +177,15 @@
   </si>
   <si>
     <t>Avg Loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy </t>
+  </si>
+  <si>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t>Hold</t>
   </si>
 </sst>
 </file>
@@ -410,11 +416,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,9 +427,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,56 +448,63 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -530,7 +537,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>1038246</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>177523</xdr:rowOff>
+      <xdr:rowOff>169963</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -885,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29739BC-04EA-4923-93C9-091C57CFB12F}">
   <dimension ref="B2:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I3" zoomScale="91" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="63" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -910,511 +917,541 @@
   <sheetData>
     <row r="2" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="27"/>
     </row>
     <row r="4" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="17">
         <v>0.82288300000000003</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="16">
         <v>2.5709999999999999E-3</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="16">
         <v>16.437384000000002</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="17">
         <v>15.494300000000001</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="18">
         <v>0.94308400000000003</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="O5" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="19"/>
-      <c r="O5" s="17" t="s">
+      <c r="P5" s="27"/>
+      <c r="R5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="19"/>
-      <c r="R5" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="S5" s="19"/>
+      <c r="S5" s="27"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="21">
         <v>0.82557899999999995</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="20">
         <v>5.7600000000000004E-3</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="20">
         <v>15.815614999999999</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="21">
         <v>15.494300000000001</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="22">
         <v>0.32131500000000002</v>
       </c>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="20"/>
+      <c r="O6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="20"/>
+      <c r="R6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" s="20"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="21">
+        <v>0.92418299999999998</v>
+      </c>
+      <c r="E7" s="20">
+        <v>8.1960000000000002E-3</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="20">
+        <v>16.677340000000001</v>
+      </c>
+      <c r="H7" s="21">
+        <v>15.494300000000001</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="22">
+        <v>1.1830400000000001</v>
+      </c>
+      <c r="L7" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="25"/>
-      <c r="O6" s="24" t="s">
+      <c r="M7" s="20"/>
+      <c r="O7" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="25"/>
-      <c r="R6" s="24" t="s">
+      <c r="P7" s="20"/>
+      <c r="R7" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="S6" s="25"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B7" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="26">
-        <v>0.92418299999999998</v>
-      </c>
-      <c r="E7" s="25">
-        <v>8.1960000000000002E-3</v>
-      </c>
-      <c r="F7" s="26" t="s">
+      <c r="S7" s="20"/>
+    </row>
+    <row r="8" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="21">
+        <v>0.97918799999999995</v>
+      </c>
+      <c r="E8" s="20">
+        <v>8.4690000000000008E-3</v>
+      </c>
+      <c r="F8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="25">
-        <v>16.677340000000001</v>
-      </c>
-      <c r="H7" s="26">
+      <c r="G8" s="20">
+        <v>23.084959999999999</v>
+      </c>
+      <c r="H8" s="21">
         <v>15.494300000000001</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="27">
-        <v>1.1830400000000001</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="25"/>
-      <c r="O7" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="P7" s="25"/>
-      <c r="R7" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="S7" s="25"/>
-    </row>
-    <row r="8" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="26">
-        <v>0.97918799999999995</v>
-      </c>
-      <c r="E8" s="25">
-        <v>8.4690000000000008E-3</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="25">
-        <v>23.084959999999999</v>
-      </c>
-      <c r="H8" s="26">
-        <v>15.494300000000001</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="27">
+      <c r="J8" s="22">
         <v>7.5906599999999997</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="M8" s="25"/>
       <c r="O8" s="24" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="P8" s="25"/>
       <c r="R8" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="S8" s="25"/>
+    </row>
+    <row r="9" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.98964200000000002</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1.0649E-2</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="12">
+        <v>26.649989000000001</v>
+      </c>
+      <c r="H9" s="13">
+        <v>15.494300000000001</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="14">
+        <v>11.155689000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.75564900000000002</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.5070999999999999E-2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="4">
+        <v>16.157188000000001</v>
+      </c>
+      <c r="H10" s="3">
+        <v>15.494300000000001</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.66288800000000003</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="27"/>
+      <c r="O10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" s="27"/>
+      <c r="R10" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="27"/>
+    </row>
+    <row r="11" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L11" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="L12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="16"/>
+      <c r="O12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="P12" s="16"/>
+      <c r="R12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S12" s="16"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="L13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="20"/>
+      <c r="O13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="20"/>
+      <c r="R13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" s="20"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="L14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="20"/>
+      <c r="O14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14" s="20"/>
+      <c r="R14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="S14" s="20"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="L15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="20"/>
+      <c r="O15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15" s="20"/>
+      <c r="R15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="S15" s="20"/>
+    </row>
+    <row r="16" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L16" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="25"/>
+      <c r="O16" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="S16" s="25"/>
+    </row>
+    <row r="17" spans="12:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="18" spans="12:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L18" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="S8" s="25"/>
-    </row>
-    <row r="9" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="15">
-        <v>0.98964200000000002</v>
-      </c>
-      <c r="E9" s="14">
-        <v>1.0649E-2</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="14">
-        <v>26.649989000000001</v>
-      </c>
-      <c r="H9" s="15">
-        <v>15.494300000000001</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="16">
-        <v>11.155689000000001</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="M9" s="30"/>
-      <c r="O9" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="P9" s="30"/>
-      <c r="R9" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="S9" s="30"/>
-    </row>
-    <row r="10" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.75564900000000002</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1.5070999999999999E-2</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="6">
-        <v>16.157188000000001</v>
-      </c>
-      <c r="H10" s="4">
-        <v>15.494300000000001</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0.66288800000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="L11" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="19"/>
-      <c r="O11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="P11" s="19"/>
-      <c r="R11" s="17" t="s">
+      <c r="M18" s="27"/>
+      <c r="O18" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="P18" s="27"/>
+      <c r="R18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="S18" s="27"/>
+    </row>
+    <row r="19" spans="12:19" x14ac:dyDescent="0.45">
+      <c r="L19" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="16"/>
+      <c r="O19" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="S19" s="16"/>
+    </row>
+    <row r="20" spans="12:19" x14ac:dyDescent="0.45">
+      <c r="L20" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="M20" s="20"/>
+      <c r="O20" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="S20" s="20"/>
+    </row>
+    <row r="21" spans="12:19" x14ac:dyDescent="0.45">
+      <c r="L21" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="M21" s="20"/>
+      <c r="O21" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="S21" s="20"/>
+    </row>
+    <row r="22" spans="12:19" x14ac:dyDescent="0.45">
+      <c r="L22" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="M22" s="20"/>
+      <c r="O22" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="S22" s="20"/>
+    </row>
+    <row r="23" spans="12:19" x14ac:dyDescent="0.45">
+      <c r="L23" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M23" s="20"/>
+      <c r="O23" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="S23" s="20"/>
+    </row>
+    <row r="24" spans="12:19" x14ac:dyDescent="0.45">
+      <c r="L24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="M24" s="20"/>
+      <c r="O24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="S24" s="20"/>
+    </row>
+    <row r="25" spans="12:19" x14ac:dyDescent="0.45">
+      <c r="L25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="S11" s="19"/>
-    </row>
-    <row r="12" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="L12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="R12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="S12" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="L13" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="21"/>
-      <c r="O13" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="P13" s="21"/>
-      <c r="R13" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="S13" s="21"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="L14" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="25"/>
-      <c r="O14" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" s="25"/>
-      <c r="R14" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="S14" s="25"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="L15" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="25"/>
-      <c r="O15" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="P15" s="25"/>
-      <c r="R15" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="S15" s="25"/>
-    </row>
-    <row r="16" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="L16" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16" s="30"/>
-      <c r="O16" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="P16" s="30"/>
-      <c r="R16" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="S16" s="30"/>
-    </row>
-    <row r="18" spans="12:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="19" spans="12:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="L19" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M19" s="19"/>
-      <c r="O19" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="P19" s="19"/>
-      <c r="R19" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="S19" s="19"/>
-    </row>
-    <row r="20" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L20" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="M20" s="21"/>
-      <c r="O20" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="P20" s="21"/>
-      <c r="R20" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="S20" s="21"/>
-    </row>
-    <row r="21" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L21" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="M21" s="25"/>
-      <c r="O21" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="P21" s="25"/>
-      <c r="R21" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="S21" s="25"/>
-    </row>
-    <row r="22" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M22" s="5"/>
-      <c r="O22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P22" s="5"/>
-      <c r="R22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S22" s="5"/>
-    </row>
-    <row r="23" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L23" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="M23" s="25"/>
-      <c r="O23" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="P23" s="25"/>
-      <c r="R23" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="S23" s="25"/>
-    </row>
-    <row r="24" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L24" s="24" t="s">
+      <c r="M25" s="20"/>
+      <c r="O25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S25" s="20"/>
+    </row>
+    <row r="26" spans="12:19" x14ac:dyDescent="0.45">
+      <c r="L26" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26" s="20"/>
+      <c r="O26" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="S26" s="20"/>
+    </row>
+    <row r="27" spans="12:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L27" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="M24" s="25"/>
-      <c r="O24" s="24" t="s">
+      <c r="M27" s="25"/>
+      <c r="O27" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="P24" s="25"/>
-      <c r="R24" s="24" t="s">
+      <c r="P27" s="25"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="S24" s="25"/>
-    </row>
-    <row r="25" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L25" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="M25" s="25"/>
-      <c r="O25" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="P25" s="25"/>
-      <c r="R25" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="S25" s="25"/>
-    </row>
-    <row r="26" spans="12:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="L26" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="M26" s="30"/>
-      <c r="O26" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="P26" s="30"/>
-      <c r="R26" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="S26" s="30"/>
-    </row>
-    <row r="27" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
+      <c r="S27" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="B3:J3"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="R5:S5"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="R10:S10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor configuration parameters, enhance metrics calculations, and improve visualization aesthetics
</commit_message>
<xml_diff>
--- a/004 tables.xlsx
+++ b/004 tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ppmel\Documentos\ITESO 7mo Semestre\004-Kalman-Filter-Implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCDE9B8-E04A-44CE-AF95-3293A647CCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162142D3-7CFF-4CD0-9B80-61F634CCC204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{920A4843-AD7D-4180-9CF4-44E3616DB8A7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{920A4843-AD7D-4180-9CF4-44E3616DB8A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="57">
   <si>
     <t>PAIR SELECTION</t>
   </si>
@@ -186,13 +186,38 @@
   </si>
   <si>
     <t>Hold</t>
+  </si>
+  <si>
+    <t>Eigenvector_1</t>
+  </si>
+  <si>
+    <t>Eigenvector_2</t>
+  </si>
+  <si>
+    <t>Beta1_norm</t>
+  </si>
+  <si>
+    <t>Beta2_norm</t>
+  </si>
+  <si>
+    <t>AMZN</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>AMD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +229,27 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -413,23 +459,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,9 +484,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -478,13 +511,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -492,12 +521,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -507,9 +530,54 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="173" fontId="0" fillId="4" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -522,55 +590,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1038246</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>169963</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46EDABD9-BFA2-9BBB-A1C4-41FB42B11306}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3195637" y="2857500"/>
-          <a:ext cx="2981347" cy="1533536"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -890,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29739BC-04EA-4923-93C9-091C57CFB12F}">
-  <dimension ref="B2:S27"/>
+  <dimension ref="B2:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="63" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -907,553 +926,1060 @@
     <col min="8" max="8" width="15.265625" customWidth="1"/>
     <col min="9" max="9" width="20.53125" customWidth="1"/>
     <col min="10" max="10" width="18.46484375" customWidth="1"/>
-    <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="16.1328125" customWidth="1"/>
-    <col min="15" max="15" width="20.9296875" customWidth="1"/>
-    <col min="16" max="16" width="15.3984375" customWidth="1"/>
-    <col min="18" max="18" width="20.53125" customWidth="1"/>
-    <col min="19" max="19" width="15.1328125" customWidth="1"/>
+    <col min="11" max="11" width="14.73046875" customWidth="1"/>
+    <col min="12" max="12" width="14.46484375" style="33" customWidth="1"/>
+    <col min="13" max="13" width="13.796875" style="33" customWidth="1"/>
+    <col min="14" max="14" width="17.86328125" style="33" customWidth="1"/>
+    <col min="15" max="18" width="10.6640625" style="33"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="16.1328125" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.9296875" customWidth="1"/>
+    <col min="23" max="23" width="15.3984375" customWidth="1"/>
+    <col min="25" max="25" width="20.53125" customWidth="1"/>
+    <col min="26" max="26" width="15.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="26" t="s">
+    <row r="2" spans="2:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="U2" s="28"/>
+    </row>
+    <row r="3" spans="2:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="27"/>
-    </row>
-    <row r="4" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="7" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="24"/>
+    </row>
+    <row r="4" spans="2:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="15" t="s">
+    <row r="5" spans="2:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="17">
-        <v>0.82288300000000003</v>
-      </c>
-      <c r="E5" s="16">
-        <v>2.5709999999999999E-3</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="16">
-        <v>16.437384000000002</v>
-      </c>
-      <c r="H5" s="17">
+      <c r="D5" s="12">
+        <v>0.82245400000000002</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2.6459999999999999E-3</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="11">
+        <v>16.341964000000001</v>
+      </c>
+      <c r="H5" s="12">
         <v>15.494300000000001</v>
       </c>
-      <c r="I5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="18">
-        <v>0.94308400000000003</v>
-      </c>
-      <c r="L5" s="26" t="s">
+      <c r="I5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0.43406800000000001</v>
+      </c>
+      <c r="K5" s="11">
+        <v>-1.3795999999999999E-2</v>
+      </c>
+      <c r="L5" s="12">
+        <v>-31.463381999999999</v>
+      </c>
+      <c r="M5" s="11">
+        <v>1</v>
+      </c>
+      <c r="N5" s="13">
+        <v>0.84766399999999997</v>
+      </c>
+      <c r="S5" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="27"/>
-      <c r="O5" s="26" t="s">
+      <c r="T5" s="24"/>
+      <c r="V5" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="P5" s="27"/>
-      <c r="R5" s="26" t="s">
+      <c r="W5" s="24"/>
+      <c r="Y5" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="S5" s="27"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B6" s="19" t="s">
+      <c r="Z5" s="24"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.45">
+      <c r="B6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="21">
-        <v>0.82557899999999995</v>
-      </c>
-      <c r="E6" s="20">
-        <v>5.7600000000000004E-3</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="20">
-        <v>15.815614999999999</v>
-      </c>
-      <c r="H6" s="21">
+      <c r="D6" s="35">
+        <v>0.82575600000000005</v>
+      </c>
+      <c r="E6" s="15">
+        <v>5.6899999999999997E-3</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="15">
+        <v>15.781355</v>
+      </c>
+      <c r="H6" s="35">
         <v>15.494300000000001</v>
       </c>
-      <c r="I6" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="22">
-        <v>0.32131500000000002</v>
-      </c>
-      <c r="L6" s="19" t="s">
+      <c r="I6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="35">
+        <v>9.6196000000000004E-2</v>
+      </c>
+      <c r="K6" s="15">
+        <v>-6.0082000000000003E-2</v>
+      </c>
+      <c r="L6" s="35">
+        <v>-1.6010819999999999</v>
+      </c>
+      <c r="M6" s="15">
+        <v>1</v>
+      </c>
+      <c r="N6" s="16">
+        <v>0.287055</v>
+      </c>
+      <c r="S6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="20"/>
-      <c r="O6" s="19" t="s">
+      <c r="T6" s="27">
+        <v>1000000</v>
+      </c>
+      <c r="V6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="P6" s="20"/>
-      <c r="R6" s="19" t="s">
+      <c r="W6" s="27">
+        <v>1000000</v>
+      </c>
+      <c r="Y6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="S6" s="20"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B7" s="19" t="s">
+      <c r="Z6" s="27">
+        <v>1538861</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.45">
+      <c r="B7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="35">
+        <v>0.93362000000000001</v>
+      </c>
+      <c r="E7" s="15">
+        <v>6.2940000000000001E-3</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="15">
+        <v>16.684159000000001</v>
+      </c>
+      <c r="H7" s="35">
+        <v>15.494300000000001</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="35">
+        <v>7.6033000000000003E-2</v>
+      </c>
+      <c r="K7" s="15">
+        <v>-9.9863999999999994E-2</v>
+      </c>
+      <c r="L7" s="35">
+        <v>-0.76136400000000004</v>
+      </c>
+      <c r="M7" s="15">
+        <v>1</v>
+      </c>
+      <c r="N7" s="16">
+        <v>1.189859</v>
+      </c>
+      <c r="S7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7" s="27">
+        <v>881509.97</v>
+      </c>
+      <c r="V7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="27">
+        <v>1538861</v>
+      </c>
+      <c r="Y7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z7" s="27">
+        <v>2077107</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="21">
-        <v>0.92418299999999998</v>
-      </c>
-      <c r="E7" s="20">
-        <v>8.1960000000000002E-3</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="20">
-        <v>16.677340000000001</v>
-      </c>
-      <c r="H7" s="21">
+      <c r="D8" s="35">
+        <v>0.92437100000000005</v>
+      </c>
+      <c r="E8" s="15">
+        <v>8.352E-3</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="15">
+        <v>16.717766999999998</v>
+      </c>
+      <c r="H8" s="35">
         <v>15.494300000000001</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="22">
-        <v>1.1830400000000001</v>
-      </c>
-      <c r="L7" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="20"/>
-      <c r="O7" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P7" s="20"/>
-      <c r="R7" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="20"/>
-    </row>
-    <row r="8" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="19" t="s">
+      <c r="I8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="35">
+        <v>0.12947400000000001</v>
+      </c>
+      <c r="K8" s="15">
+        <v>-8.2418000000000005E-2</v>
+      </c>
+      <c r="L8" s="35">
+        <v>-1.5709470000000001</v>
+      </c>
+      <c r="M8" s="15">
+        <v>1</v>
+      </c>
+      <c r="N8" s="16">
+        <v>1.2234670000000001</v>
+      </c>
+      <c r="S8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="26">
+        <v>-0.11849999999999999</v>
+      </c>
+      <c r="V8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="W8" s="31">
+        <v>0.53890000000000005</v>
+      </c>
+      <c r="Y8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z8" s="31">
+        <v>0.3498</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C9" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="21">
-        <v>0.97918799999999995</v>
-      </c>
-      <c r="E8" s="20">
-        <v>8.4690000000000008E-3</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="20">
-        <v>23.084959999999999</v>
-      </c>
-      <c r="H8" s="21">
+      <c r="D9" s="8">
+        <v>0.97917299999999996</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1.0406E-2</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="7">
+        <v>22.095528000000002</v>
+      </c>
+      <c r="H9" s="8">
         <v>15.494300000000001</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="22">
-        <v>7.5906599999999997</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="25"/>
-      <c r="O8" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="P8" s="25"/>
-      <c r="R8" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="S8" s="25"/>
-    </row>
-    <row r="9" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="11" t="s">
+      <c r="I9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.31404599999999999</v>
+      </c>
+      <c r="K9" s="7">
+        <v>-8.8092000000000004E-2</v>
+      </c>
+      <c r="L9" s="8">
+        <v>-3.5649709999999999</v>
+      </c>
+      <c r="M9" s="7">
+        <v>1</v>
+      </c>
+      <c r="N9" s="9">
+        <v>6.6012279999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="35">
+        <v>0.94392600000000004</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1.2147E-2</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="15">
+        <v>15.703646000000001</v>
+      </c>
+      <c r="H10" s="35">
+        <v>15.494300000000001</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="35">
+        <v>3.6814E-2</v>
+      </c>
+      <c r="K10" s="15">
+        <v>-0.113524</v>
+      </c>
+      <c r="L10" s="35">
+        <v>-0.32428400000000002</v>
+      </c>
+      <c r="M10" s="15">
+        <v>1</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0.209346</v>
+      </c>
+      <c r="S10" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="T10" s="24"/>
+      <c r="V10" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="W10" s="24"/>
+      <c r="Y10" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z10" s="24"/>
+    </row>
+    <row r="11" spans="2:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="35">
+        <v>0.93024700000000005</v>
+      </c>
+      <c r="E11" s="15">
+        <v>1.2409999999999999E-2</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="15">
+        <v>18.711338999999999</v>
+      </c>
+      <c r="H11" s="35">
+        <v>15.494300000000001</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="35">
+        <v>0.15828400000000001</v>
+      </c>
+      <c r="K11" s="15">
+        <v>-0.134662</v>
+      </c>
+      <c r="L11" s="35">
+        <v>-1.175416</v>
+      </c>
+      <c r="M11" s="15">
+        <v>1</v>
+      </c>
+      <c r="N11" s="16">
+        <v>3.2170390000000002</v>
+      </c>
+      <c r="S11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="T11" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.45">
+      <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="13">
-        <v>0.98964200000000002</v>
-      </c>
-      <c r="E9" s="12">
-        <v>1.0649E-2</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="12">
-        <v>26.649989000000001</v>
-      </c>
-      <c r="H9" s="13">
+      <c r="D12" s="35">
+        <v>0.98962499999999998</v>
+      </c>
+      <c r="E12" s="15">
+        <v>1.3112E-2</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="15">
+        <v>25.437892999999999</v>
+      </c>
+      <c r="H12" s="35">
         <v>15.494300000000001</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="14">
-        <v>11.155689000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="1" t="s">
+      <c r="I12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="35">
+        <v>0.14650199999999999</v>
+      </c>
+      <c r="K12" s="15">
+        <v>-8.1119999999999998E-2</v>
+      </c>
+      <c r="L12" s="35">
+        <v>-1.8059829999999999</v>
+      </c>
+      <c r="M12" s="15">
+        <v>1</v>
+      </c>
+      <c r="N12" s="16">
+        <v>9.9435929999999999</v>
+      </c>
+      <c r="S12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="T12" s="11">
+        <f>-0.1627</f>
+        <v>-0.16270000000000001</v>
+      </c>
+      <c r="V12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="W12" s="11">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="Y12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z12" s="11">
+        <v>0.85570000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.45">
+      <c r="B13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="3">
-        <v>0.75564900000000002</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1.5070999999999999E-2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="4">
-        <v>16.157188000000001</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="D13" s="35">
+        <v>0.75515100000000002</v>
+      </c>
+      <c r="E13" s="15">
+        <v>1.7087000000000001E-2</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="15">
+        <v>15.923693999999999</v>
+      </c>
+      <c r="H13" s="35">
         <v>15.494300000000001</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.66288800000000003</v>
-      </c>
-      <c r="L10" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="27"/>
-      <c r="O10" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="P10" s="27"/>
-      <c r="R10" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="S10" s="27"/>
-    </row>
-    <row r="11" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="L11" s="30" t="s">
+      <c r="I13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="35">
+        <v>4.7111E-2</v>
+      </c>
+      <c r="K13" s="15">
+        <v>-6.9278999999999993E-2</v>
+      </c>
+      <c r="L13" s="35">
+        <v>-0.68002300000000004</v>
+      </c>
+      <c r="M13" s="15">
+        <v>1</v>
+      </c>
+      <c r="N13" s="16">
+        <v>0.429394</v>
+      </c>
+      <c r="S13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" s="15">
+        <v>-7.2300000000000003E-2</v>
+      </c>
+      <c r="V13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="W13" s="15">
+        <v>0.72060000000000002</v>
+      </c>
+      <c r="Y13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z13" s="15">
+        <v>0.93420000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.45">
+      <c r="B14" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="35">
+        <v>0.94259700000000002</v>
+      </c>
+      <c r="E14" s="15">
+        <v>2.7163E-2</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="15">
+        <v>17.178049999999999</v>
+      </c>
+      <c r="H14" s="35">
+        <v>15.494300000000001</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="35">
+        <v>0.13022500000000001</v>
+      </c>
+      <c r="K14" s="15">
+        <v>-3.4074E-2</v>
+      </c>
+      <c r="L14" s="35">
+        <v>-3.8218070000000002</v>
+      </c>
+      <c r="M14" s="15">
+        <v>1</v>
+      </c>
+      <c r="N14" s="16">
+        <v>1.6837500000000001</v>
+      </c>
+      <c r="S14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="T14" s="15">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="V14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="W14" s="15">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="Y14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z14" s="15">
+        <v>0.2394</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="37">
+        <v>0.85282999999999998</v>
+      </c>
+      <c r="E15" s="18">
+        <v>2.7328000000000002E-2</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="18">
+        <v>15.646011</v>
+      </c>
+      <c r="H15" s="37">
+        <v>15.494300000000001</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="37">
+        <v>8.5572999999999996E-2</v>
+      </c>
+      <c r="K15" s="18">
+        <v>-0.10408000000000001</v>
+      </c>
+      <c r="L15" s="37">
+        <v>-0.82218400000000003</v>
+      </c>
+      <c r="M15" s="18">
+        <v>1</v>
+      </c>
+      <c r="N15" s="38">
+        <v>0.15171100000000001</v>
+      </c>
+      <c r="S15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="T15" s="15">
+        <v>-4.4299999999999999E-2</v>
+      </c>
+      <c r="V15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="W15" s="15">
+        <v>1.8875999999999999</v>
+      </c>
+      <c r="Y15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z15" s="15">
+        <v>0.4763</v>
+      </c>
+    </row>
+    <row r="16" spans="2:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="S16" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="T16" s="34">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="V16" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="W16" s="18">
+        <v>0.1009</v>
+      </c>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z16" s="18">
+        <v>0.15890000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+    </row>
+    <row r="18" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="S18" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="T18" s="24"/>
+      <c r="V18" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="W18" s="24"/>
+      <c r="Y18" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z18" s="24"/>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="S19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="T19" s="11">
+        <v>60</v>
+      </c>
+      <c r="V19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="W19" s="11">
+        <v>44</v>
+      </c>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z19" s="11">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="S20" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="T20" s="15">
+        <v>30</v>
+      </c>
+      <c r="V20" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="W20" s="15">
         <v>23</v>
       </c>
-      <c r="M11" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S11" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="L12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="16"/>
-      <c r="O12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="16"/>
-      <c r="R12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="S12" s="16"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="L13" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="20"/>
-      <c r="O13" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="20"/>
-      <c r="R13" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="S13" s="20"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="L14" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="20"/>
-      <c r="O14" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="P14" s="20"/>
-      <c r="R14" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="S14" s="20"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="L15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="M15" s="20"/>
-      <c r="O15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="P15" s="20"/>
-      <c r="R15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="S15" s="20"/>
-    </row>
-    <row r="16" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="L16" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="M16" s="25"/>
-      <c r="O16" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="S16" s="25"/>
-    </row>
-    <row r="17" spans="12:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="18" spans="12:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="L18" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="M18" s="27"/>
-      <c r="O18" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="P18" s="27"/>
-      <c r="R18" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="S18" s="27"/>
-    </row>
-    <row r="19" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L19" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19" s="16"/>
-      <c r="O19" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="S19" s="16"/>
-    </row>
-    <row r="20" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L20" s="19" t="s">
+      <c r="X20" s="20"/>
+      <c r="Y20" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="M20" s="20"/>
-      <c r="O20" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="S20" s="20"/>
-    </row>
-    <row r="21" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L21" s="19" t="s">
+      <c r="Z20" s="15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="S21" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="M21" s="20"/>
-      <c r="O21" s="19" t="s">
+      <c r="T21" s="15">
+        <v>60</v>
+      </c>
+      <c r="V21" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="19" t="s">
+      <c r="W21" s="15">
+        <v>44</v>
+      </c>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="S21" s="20"/>
-    </row>
-    <row r="22" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L22" s="19" t="s">
+      <c r="Z21" s="15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="S22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="M22" s="20"/>
-      <c r="O22" s="19" t="s">
+      <c r="T22" s="15">
+        <v>1771</v>
+      </c>
+      <c r="V22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="19" t="s">
+      <c r="W22" s="15">
+        <v>593</v>
+      </c>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="S22" s="20"/>
-    </row>
-    <row r="23" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L23" s="19" t="s">
+      <c r="Z22" s="15">
+        <v>600</v>
+      </c>
+      <c r="AB22" s="32"/>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="S23" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="M23" s="20"/>
-      <c r="O23" s="19" t="s">
+      <c r="T23" s="27">
+        <v>17244.400000000001</v>
+      </c>
+      <c r="V23" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="19" t="s">
+      <c r="W23" s="27">
+        <v>39667.74</v>
+      </c>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="S23" s="20"/>
-    </row>
-    <row r="24" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L24" s="19" t="s">
+      <c r="Z23" s="27">
+        <v>40131.760000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="S24" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="M24" s="20"/>
-      <c r="O24" s="19" t="s">
+      <c r="T24" s="27">
+        <v>-21100</v>
+      </c>
+      <c r="V24" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="29"/>
-      <c r="R24" s="19" t="s">
+      <c r="W24" s="27">
+        <v>-28759.599999999999</v>
+      </c>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="S24" s="20"/>
-    </row>
-    <row r="25" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L25" s="19" t="s">
+      <c r="Z24" s="27">
+        <v>-42607.3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="S25" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="M25" s="20"/>
-      <c r="O25" s="19" t="s">
+      <c r="T25" s="29">
+        <f>T7-T6</f>
+        <v>-118490.03000000003</v>
+      </c>
+      <c r="V25" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="19" t="s">
+      <c r="W25" s="27">
+        <v>582116</v>
+      </c>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="S25" s="20"/>
-    </row>
-    <row r="26" spans="12:19" x14ac:dyDescent="0.45">
-      <c r="L26" s="19" t="s">
+      <c r="Z25" s="27">
+        <v>585169.6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="S26" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="M26" s="20"/>
-      <c r="O26" s="19" t="s">
+      <c r="T26" s="27">
+        <v>1956.1</v>
+      </c>
+      <c r="V26" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="29"/>
-      <c r="R26" s="19" t="s">
+      <c r="W26" s="27">
+        <v>1517.54</v>
+      </c>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="S26" s="20"/>
-    </row>
-    <row r="27" spans="12:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="L27" s="24" t="s">
+      <c r="Z26" s="27">
+        <v>2759.51</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="S27" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="M27" s="25"/>
-      <c r="O27" s="24" t="s">
+      <c r="T27" s="30">
+        <v>105488.68</v>
+      </c>
+      <c r="V27" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="29"/>
-      <c r="R27" s="24" t="s">
+      <c r="W27" s="30">
+        <v>118942.9</v>
+      </c>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="S27" s="25"/>
+      <c r="Z27" s="30">
+        <v>181049.3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="B3:N3"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>